<commit_message>
"[insert] kakao api를 활용한 테스트"
</commit_message>
<xml_diff>
--- a/논리 데이터 모델링 참고.xlsx
+++ b/논리 데이터 모델링 참고.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java2\teamproject-workspace\MaumgagymProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD152DD-6B0C-4E66-B5E9-2B5F730E6708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FED8390-4280-4A61-9338-FB021A4D4D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{2A184F4F-55DA-4D87-8CCE-16812E380CA2}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{2A184F4F-55DA-4D87-8CCE-16812E380CA2}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="146">
   <si>
     <t>글 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,10 +175,6 @@
   </si>
   <si>
     <t>공지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>글 태그</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1320,8 +1316,8 @@
   </sheetPr>
   <dimension ref="C1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1363,10 +1359,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1383,10 +1379,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="10">
         <v>1</v>
@@ -1396,34 +1392,32 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="G5" s="5"/>
       <c r="J5" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="3:14" ht="24" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>145</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1431,16 +1425,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" s="10">
         <v>1</v>
@@ -1454,16 +1448,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" s="10">
         <v>2</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="10">
         <v>1</v>
@@ -1477,16 +1471,16 @@
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="10">
         <v>3</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" s="10">
         <v>1</v>
@@ -1500,16 +1494,16 @@
         <v>4</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="10">
         <v>4</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="10">
         <v>1</v>
@@ -1523,10 +1517,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J11" s="10">
         <v>2</v>
@@ -1540,13 +1534,13 @@
         <v>6</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1556,34 +1550,34 @@
         <v>7</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H13" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="K13" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="L13" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="M13" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="N13" s="13" t="s">
         <v>110</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1591,10 +1585,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" s="14">
         <v>1</v>
@@ -1603,7 +1597,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J14" s="3">
         <v>1234</v>
@@ -1612,13 +1606,13 @@
         <v>14</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1626,10 +1620,10 @@
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1640,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1656,22 +1650,22 @@
         <v>11</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>120</v>
-      </c>
       <c r="J17" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1679,19 +1673,19 @@
         <v>12</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="14">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J18" s="14">
         <v>1</v>
@@ -1719,10 +1713,10 @@
         <v>33</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1732,34 +1726,34 @@
         <v>15</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G21" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="L21" s="16" t="s">
+      <c r="N21" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="N21" s="17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1767,19 +1761,19 @@
         <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" s="7">
         <v>1</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>8</v>
@@ -1802,19 +1796,19 @@
         <v>17</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" s="7">
         <v>2</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>11</v>
@@ -1837,10 +1831,10 @@
         <v>3</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>13</v>
@@ -1860,10 +1854,10 @@
     </row>
     <row r="26" spans="3:14" ht="24" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -1877,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>16</v>
@@ -1889,7 +1883,7 @@
         <v>20</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>0</v>
@@ -1975,7 +1969,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -2048,7 +2042,7 @@
     </row>
     <row r="36" spans="3:14" ht="24" x14ac:dyDescent="0.3">
       <c r="C36" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -2098,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -2112,22 +2106,22 @@
         <v>3</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L40" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -2144,16 +2138,16 @@
         <v>1</v>
       </c>
       <c r="H41" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="J41" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J41" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="K41" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L41" s="10">
         <v>1</v>
@@ -2173,16 +2167,16 @@
         <v>2</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L42" s="10">
         <v>2</v>
@@ -2202,16 +2196,16 @@
         <v>3</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I43" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J43" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="K43" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="L43" s="10">
         <v>3</v>
@@ -2233,7 +2227,7 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="G45" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="3:14" ht="24" x14ac:dyDescent="0.3">
@@ -2241,25 +2235,25 @@
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="G46" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I46" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="I46" s="13" t="s">
+      <c r="J46" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="K46" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K46" s="13" t="s">
+      <c r="L46" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L46" s="13" t="s">
+      <c r="M46" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="M46" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="N46" s="13" t="s">
         <v>32</v>
@@ -2267,7 +2261,7 @@
     </row>
     <row r="47" spans="3:14" ht="24" x14ac:dyDescent="0.3">
       <c r="C47" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -2275,20 +2269,20 @@
         <v>1</v>
       </c>
       <c r="H47" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I47" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J47" s="10" t="s">
+      <c r="K47" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="K47" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="L47" s="10"/>
       <c r="M47" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N47" s="10">
         <v>1</v>
@@ -2338,7 +2332,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="3:10" ht="24" x14ac:dyDescent="0.3">
@@ -2352,16 +2346,16 @@
         <v>4</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H52" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I52" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I52" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="J52" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="3:10" ht="24" x14ac:dyDescent="0.3">
@@ -2378,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J53" s="10">
         <v>1</v>
@@ -2401,10 +2395,10 @@
         <v>2</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J54" s="10">
         <v>1</v>
@@ -2423,12 +2417,12 @@
     </row>
     <row r="57" spans="3:10" ht="24" x14ac:dyDescent="0.3">
       <c r="G57" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="3:10" ht="24" x14ac:dyDescent="0.3">
       <c r="C58" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -2438,7 +2432,7 @@
         <v>30</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E59" s="21" t="s">
         <v>15</v>
@@ -2533,7 +2527,7 @@
     </row>
     <row r="69" spans="3:5" ht="24" x14ac:dyDescent="0.3">
       <c r="C69" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -2543,7 +2537,7 @@
         <v>24</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>15</v>

</xml_diff>